<commit_message>
Changed Link toolbar button image. Moved used image files to View\Properties to hopefully fix Visual Studio resource editor 'file not found' errors
</commit_message>
<xml_diff>
--- a/Archivists' App/View/Images/_Image Sources.xlsx
+++ b/Archivists' App/View/Images/_Image Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\OneDrive\Documents\Visual Studio Projects\SoundExplorers\Archivists' App\View\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC38053E-641F-4423-B2D0-426825689552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90CE785-48DA-496D-AEFE-77C6AD619E68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{185F787C-75CB-4C6E-8AE2-88ADA4650E2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Cut Flatastic 32x32</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Link Noto Emoji 32x32</t>
+  </si>
+  <si>
+    <t>Link Cerulean 32x32</t>
+  </si>
+  <si>
+    <t>https://iconarchive.com/show/cerulean-icons-by-iconleak/link-icon.html</t>
+  </si>
+  <si>
+    <t>https://iconarchive.com/show/webuosities-icons-by-etherbrian/links-icon.html</t>
+  </si>
+  <si>
+    <t>Link Webuosities 32x32</t>
+  </si>
+  <si>
+    <t>These and others have been moved to View\Properties to try to fix Visual Studio resx editor 'file not found' errors</t>
   </si>
 </sst>
 </file>
@@ -418,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B372047D-F86E-4F80-A455-C4F35445834D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -456,10 +471,31 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +503,9 @@
     <hyperlink ref="B1" r:id="rId1" xr:uid="{350207DB-0925-4306-86A0-D41A784B49BD}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{B4F984D8-D35E-4CAB-92F2-0AD641558052}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{28CBFB52-6BA4-4640-BE02-9489C0535875}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{E2141F60-C2D4-49D8-8715-15947578773F}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{E2141F60-C2D4-49D8-8715-15947578773F}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{86757DA5-FD61-406E-9E9C-B8732EC2C704}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{7BD57134-0B66-4797-9CAD-1BC290707EB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hopefully fixed resx warnings for bitmaps properly this time, by ignoring them in Rider's solution-wide analysis
</commit_message>
<xml_diff>
--- a/Archivists' App/View/Images/_Image Sources.xlsx
+++ b/Archivists' App/View/Images/_Image Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\OneDrive\Documents\Visual Studio Projects\SoundExplorers\Archivists' App\View\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90CE785-48DA-496D-AEFE-77C6AD619E68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965F969D-8297-4D6D-94DB-75D1C1215BA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{185F787C-75CB-4C6E-8AE2-88ADA4650E2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Cut Flatastic 32x32</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Link Webuosities 32x32</t>
-  </si>
-  <si>
-    <t>These and others have been moved to View\Properties to try to fix Visual Studio resx editor 'file not found' errors</t>
   </si>
 </sst>
 </file>
@@ -433,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B372047D-F86E-4F80-A455-C4F35445834D}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -491,11 +488,6 @@
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>